<commit_message>
ready to dig the init() again
</commit_message>
<xml_diff>
--- a/Diagrams/Diagrams-1.xlsx
+++ b/Diagrams/Diagrams-1.xlsx
@@ -2270,9 +2270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2282,7 +2282,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="183960"/>
-          <a:ext cx="2004120" cy="365760"/>
+          <a:ext cx="2003400" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2340,9 +2340,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2352,7 +2352,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="552240"/>
-          <a:ext cx="2004120" cy="365760"/>
+          <a:ext cx="2003400" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2422,9 +2422,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2434,7 +2434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="920520"/>
-          <a:ext cx="2004120" cy="365760"/>
+          <a:ext cx="2003400" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2494,9 +2494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2506,7 +2506,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="1473120"/>
-          <a:ext cx="1502640" cy="365760"/>
+          <a:ext cx="1501920" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2564,9 +2564,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2576,7 +2576,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1755720" y="1473120"/>
-          <a:ext cx="1502280" cy="365760"/>
+          <a:ext cx="1501560" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2636,9 +2636,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>130680</xdr:colOff>
+      <xdr:colOff>129960</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2648,7 +2648,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3142800" y="1473120"/>
-          <a:ext cx="1502640" cy="365760"/>
+          <a:ext cx="1501920" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2708,9 +2708,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2720,7 +2720,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="2393640"/>
-          <a:ext cx="12789720" cy="365760"/>
+          <a:ext cx="12789000" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2778,9 +2778,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2790,7 +2790,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="3130200"/>
-          <a:ext cx="12789720" cy="366120"/>
+          <a:ext cx="12789000" cy="365400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2848,9 +2848,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
-      <xdr:colOff>248040</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2860,7 +2860,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="3867120"/>
-          <a:ext cx="14043600" cy="365760"/>
+          <a:ext cx="14042880" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2918,9 +2918,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2930,7 +2930,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="4419360"/>
-          <a:ext cx="12789720" cy="734040"/>
+          <a:ext cx="12789000" cy="733320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2988,9 +2988,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
+      <xdr:colOff>9360</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3000,7 +3000,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="263160" y="5340240"/>
-          <a:ext cx="12789720" cy="365760"/>
+          <a:ext cx="12789000" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3058,9 +3058,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3070,7 +3070,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="5892480"/>
-          <a:ext cx="12789720" cy="734400"/>
+          <a:ext cx="12789000" cy="733680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3128,9 +3128,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
-      <xdr:colOff>3960</xdr:colOff>
+      <xdr:colOff>3240</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3140,7 +3140,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="257040" y="6813360"/>
-          <a:ext cx="12789720" cy="365760"/>
+          <a:ext cx="12789000" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3198,9 +3198,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3210,7 +3210,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="7365960"/>
-          <a:ext cx="12789720" cy="365760"/>
+          <a:ext cx="12789000" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3270,7 +3270,7 @@
       <xdr:col>26</xdr:col>
       <xdr:colOff>98640</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3280,7 +3280,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6619680" y="2761920"/>
-          <a:ext cx="360" cy="365760"/>
+          <a:ext cx="360" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3329,7 +3329,7 @@
       <xdr:col>26</xdr:col>
       <xdr:colOff>98640</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3339,7 +3339,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6619680" y="3498840"/>
-          <a:ext cx="360" cy="365760"/>
+          <a:ext cx="360" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3388,7 +3388,7 @@
       <xdr:col>26</xdr:col>
       <xdr:colOff>98640</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3398,7 +3398,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6619680" y="4235400"/>
-          <a:ext cx="360" cy="181440"/>
+          <a:ext cx="360" cy="180720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3445,9 +3445,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>108360</xdr:colOff>
+      <xdr:colOff>107640</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3457,7 +3457,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6619680" y="5155920"/>
-          <a:ext cx="10080" cy="181800"/>
+          <a:ext cx="9360" cy="181080"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3498,15 +3498,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>96120</xdr:colOff>
+      <xdr:colOff>95400</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>106200</xdr:colOff>
+      <xdr:colOff>104760</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3515,8 +3515,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6617520" y="5708520"/>
-          <a:ext cx="10080" cy="181440"/>
+          <a:off x="6616800" y="5708520"/>
+          <a:ext cx="9360" cy="180720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3563,9 +3563,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>102240</xdr:colOff>
+      <xdr:colOff>101520</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3575,7 +3575,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6619680" y="6629400"/>
-          <a:ext cx="3960" cy="181440"/>
+          <a:ext cx="3240" cy="180720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3616,15 +3616,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>95400</xdr:colOff>
+      <xdr:colOff>94680</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>99360</xdr:colOff>
+      <xdr:colOff>97920</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3633,8 +3633,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6616800" y="7181640"/>
-          <a:ext cx="3960" cy="181800"/>
+          <a:off x="6616080" y="7181640"/>
+          <a:ext cx="3240" cy="181080"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3681,9 +3681,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3693,7 +3693,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="8464320"/>
-          <a:ext cx="12789720" cy="365760"/>
+          <a:ext cx="12789000" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3751,9 +3751,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>223920</xdr:colOff>
+      <xdr:colOff>223200</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3763,7 +3763,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="226440" y="9016920"/>
-          <a:ext cx="12789360" cy="365760"/>
+          <a:ext cx="12788640" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3815,15 +3815,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>89280</xdr:colOff>
+      <xdr:colOff>88560</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>177840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>93240</xdr:colOff>
+      <xdr:colOff>91800</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3832,8 +3832,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6610680" y="8832600"/>
-          <a:ext cx="3960" cy="181800"/>
+          <a:off x="6609960" y="8832600"/>
+          <a:ext cx="3240" cy="181080"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3880,9 +3880,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3892,7 +3892,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="9943920"/>
-          <a:ext cx="4010760" cy="365760"/>
+          <a:ext cx="4010040" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -3950,9 +3950,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3962,7 +3962,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="269640" y="10699560"/>
-          <a:ext cx="4010760" cy="365760"/>
+          <a:ext cx="4010040" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -4020,9 +4020,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4032,7 +4032,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="11417040"/>
-          <a:ext cx="4010760" cy="365760"/>
+          <a:ext cx="4010040" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -4090,9 +4090,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4102,7 +4102,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="269640" y="12172680"/>
-          <a:ext cx="4010760" cy="365760"/>
+          <a:ext cx="4010040" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -4160,9 +4160,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4172,7 +4172,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="250560" y="12890160"/>
-          <a:ext cx="4010760" cy="366120"/>
+          <a:ext cx="4010040" cy="365400"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -4230,9 +4230,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>76</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4242,7 +4242,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="269640" y="13646160"/>
-          <a:ext cx="4010760" cy="365760"/>
+          <a:ext cx="4010040" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -4300,9 +4300,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4312,7 +4312,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2257200" y="10312200"/>
-          <a:ext cx="16560" cy="384840"/>
+          <a:ext cx="15840" cy="384120"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4353,15 +4353,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>248760</xdr:colOff>
+      <xdr:colOff>248040</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>19080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>14400</xdr:colOff>
+      <xdr:colOff>12960</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4370,8 +4370,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2255040" y="11067840"/>
-          <a:ext cx="16560" cy="346680"/>
+          <a:off x="2254320" y="11067840"/>
+          <a:ext cx="15840" cy="345960"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4418,9 +4418,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4430,7 +4430,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2257200" y="11785320"/>
-          <a:ext cx="16560" cy="384840"/>
+          <a:ext cx="15840" cy="384120"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4471,15 +4471,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>248760</xdr:colOff>
+      <xdr:colOff>248040</xdr:colOff>
       <xdr:row>68</xdr:row>
       <xdr:rowOff>19080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>14400</xdr:colOff>
+      <xdr:colOff>12960</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4488,8 +4488,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2255040" y="12540960"/>
-          <a:ext cx="16560" cy="346680"/>
+          <a:off x="2254320" y="12540960"/>
+          <a:ext cx="15840" cy="345960"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4536,9 +4536,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4548,7 +4548,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2257200" y="13258800"/>
-          <a:ext cx="16560" cy="384840"/>
+          <a:ext cx="15840" cy="384120"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4595,9 +4595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4607,7 +4607,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="14731920"/>
-          <a:ext cx="7522200" cy="365760"/>
+          <a:ext cx="7521480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -4665,9 +4665,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>90</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4677,7 +4677,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="15487560"/>
-          <a:ext cx="7522200" cy="1267560"/>
+          <a:ext cx="7521480" cy="1266840"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -4811,9 +4811,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>99</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4823,7 +4823,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="17145000"/>
-          <a:ext cx="7522200" cy="1267200"/>
+          <a:ext cx="7521480" cy="1266480"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -4919,9 +4919,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>103</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4931,7 +4931,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="18783000"/>
-          <a:ext cx="7522200" cy="365760"/>
+          <a:ext cx="7521480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -4999,9 +4999,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>107</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5011,7 +5011,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="19519560"/>
-          <a:ext cx="7522200" cy="366120"/>
+          <a:ext cx="7521480" cy="365400"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -5079,9 +5079,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>116</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5091,7 +5091,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="20256480"/>
-          <a:ext cx="7522200" cy="1267560"/>
+          <a:ext cx="7521480" cy="1266840"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -5225,9 +5225,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>125</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5237,7 +5237,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="21932640"/>
-          <a:ext cx="7522200" cy="1267560"/>
+          <a:ext cx="7521480" cy="1266840"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -5352,9 +5352,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>138</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5364,7 +5364,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="23590080"/>
-          <a:ext cx="7522200" cy="2004120"/>
+          <a:ext cx="7521480" cy="2003400"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -5593,9 +5593,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>146</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5605,7 +5605,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="25965000"/>
-          <a:ext cx="7522200" cy="1102320"/>
+          <a:ext cx="7521480" cy="1101600"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -5701,9 +5701,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>150</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5713,7 +5713,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="27438120"/>
-          <a:ext cx="7522200" cy="365760"/>
+          <a:ext cx="7521480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -5771,9 +5771,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>154</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5783,7 +5783,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="28174680"/>
-          <a:ext cx="7522200" cy="365760"/>
+          <a:ext cx="7521480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -5841,9 +5841,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>162</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5853,7 +5853,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="28911240"/>
-          <a:ext cx="7522200" cy="1096200"/>
+          <a:ext cx="7521480" cy="1095480"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -6016,9 +6016,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
-      <xdr:colOff>248040</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>137</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6028,7 +6028,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8277120" y="23571000"/>
-          <a:ext cx="6017040" cy="1838880"/>
+          <a:ext cx="6016320" cy="1838160"/>
         </a:xfrm>
         <a:prstGeom prst="cloudCallout">
           <a:avLst>
@@ -6129,7 +6129,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6139,7 +6139,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="15100200"/>
-          <a:ext cx="360" cy="384840"/>
+          <a:ext cx="360" cy="384120"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6188,7 +6188,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>92</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6198,7 +6198,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="16757640"/>
-          <a:ext cx="360" cy="365760"/>
+          <a:ext cx="360" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6247,7 +6247,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>101</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6257,7 +6257,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="18414720"/>
-          <a:ext cx="360" cy="365760"/>
+          <a:ext cx="360" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6306,7 +6306,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6316,7 +6316,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="19151280"/>
-          <a:ext cx="360" cy="365760"/>
+          <a:ext cx="360" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6365,7 +6365,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>109</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6375,7 +6375,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="19888200"/>
-          <a:ext cx="360" cy="365760"/>
+          <a:ext cx="360" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6424,7 +6424,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>118</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6434,7 +6434,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="21526560"/>
-          <a:ext cx="360" cy="384480"/>
+          <a:ext cx="360" cy="383760"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6483,7 +6483,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>127</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6493,7 +6493,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="23202720"/>
-          <a:ext cx="360" cy="365760"/>
+          <a:ext cx="360" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6542,7 +6542,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>140</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6552,7 +6552,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="25596720"/>
-          <a:ext cx="360" cy="365760"/>
+          <a:ext cx="360" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6601,7 +6601,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>148</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6611,7 +6611,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="27069840"/>
-          <a:ext cx="360" cy="365760"/>
+          <a:ext cx="360" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6660,7 +6660,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>152</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6670,7 +6670,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="27806400"/>
-          <a:ext cx="360" cy="365760"/>
+          <a:ext cx="360" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6719,7 +6719,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>156</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6729,7 +6729,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="28542960"/>
-          <a:ext cx="360" cy="365760"/>
+          <a:ext cx="360" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6776,9 +6776,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>248400</xdr:colOff>
+      <xdr:colOff>247680</xdr:colOff>
       <xdr:row>166</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6788,7 +6788,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="30384720"/>
-          <a:ext cx="7522200" cy="365760"/>
+          <a:ext cx="7521480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -6848,7 +6848,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>360</xdr:colOff>
       <xdr:row>164</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6858,7 +6858,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4263840" y="30009960"/>
-          <a:ext cx="360" cy="372240"/>
+          <a:ext cx="360" cy="371520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6907,7 +6907,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>190800</xdr:colOff>
       <xdr:row>169</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6917,7 +6917,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4203360" y="30759480"/>
-          <a:ext cx="360" cy="372240"/>
+          <a:ext cx="360" cy="371520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6964,9 +6964,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>3960</xdr:colOff>
+      <xdr:colOff>3240</xdr:colOff>
       <xdr:row>171</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6976,7 +6976,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="507960" y="31140360"/>
-          <a:ext cx="7522200" cy="365760"/>
+          <a:ext cx="7521480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -7036,7 +7036,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>6840</xdr:colOff>
       <xdr:row>173</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7046,7 +7046,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4270320" y="31496040"/>
-          <a:ext cx="360" cy="372240"/>
+          <a:ext cx="360" cy="371520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7093,9 +7093,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>175</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7105,7 +7105,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="520560" y="31876920"/>
-          <a:ext cx="7522200" cy="365760"/>
+          <a:ext cx="7521480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -7165,7 +7165,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>190800</xdr:colOff>
       <xdr:row>177</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7175,7 +7175,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4203360" y="32238720"/>
-          <a:ext cx="360" cy="372240"/>
+          <a:ext cx="360" cy="371520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7222,9 +7222,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>3960</xdr:colOff>
+      <xdr:colOff>3240</xdr:colOff>
       <xdr:row>179</xdr:row>
-      <xdr:rowOff>23040</xdr:rowOff>
+      <xdr:rowOff>22320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7234,7 +7234,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="507960" y="32619960"/>
-          <a:ext cx="7522200" cy="365760"/>
+          <a:ext cx="7521480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -7302,9 +7302,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>187920</xdr:colOff>
+      <xdr:colOff>187200</xdr:colOff>
       <xdr:row>183</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7314,7 +7314,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="441000" y="33337440"/>
-          <a:ext cx="7522200" cy="365760"/>
+          <a:ext cx="7521480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -7366,15 +7366,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>188280</xdr:colOff>
+      <xdr:colOff>187560</xdr:colOff>
       <xdr:row>179</xdr:row>
       <xdr:rowOff>25560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>250920</xdr:colOff>
       <xdr:row>181</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7383,8 +7383,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4201200" y="32988240"/>
-          <a:ext cx="64080" cy="346680"/>
+          <a:off x="4200480" y="32988240"/>
+          <a:ext cx="63360" cy="345960"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7431,9 +7431,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>168840</xdr:colOff>
+      <xdr:colOff>168120</xdr:colOff>
       <xdr:row>188</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7443,7 +7443,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="441000" y="34264440"/>
-          <a:ext cx="3490200" cy="365760"/>
+          <a:ext cx="3489480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -7495,15 +7495,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>178200</xdr:colOff>
+      <xdr:colOff>177480</xdr:colOff>
       <xdr:row>183</xdr:row>
       <xdr:rowOff>6480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>245520</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>186</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7512,8 +7512,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2184480" y="33705720"/>
-          <a:ext cx="67320" cy="556560"/>
+          <a:off x="2183760" y="33705720"/>
+          <a:ext cx="66600" cy="555840"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7560,9 +7560,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>187920</xdr:colOff>
+      <xdr:colOff>187200</xdr:colOff>
       <xdr:row>188</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7572,7 +7572,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4777920" y="34264440"/>
-          <a:ext cx="3436200" cy="365760"/>
+          <a:ext cx="3435480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -7629,10 +7629,10 @@
       <xdr:rowOff>6480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>250920</xdr:colOff>
       <xdr:row>186</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7642,7 +7642,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2196720" y="33890040"/>
-          <a:ext cx="4325400" cy="372240"/>
+          <a:ext cx="4324680" cy="371520"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -7676,9 +7676,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>175320</xdr:colOff>
+      <xdr:colOff>174600</xdr:colOff>
       <xdr:row>192</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7688,7 +7688,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="501480" y="35001000"/>
-          <a:ext cx="3436200" cy="365760"/>
+          <a:ext cx="3435480" cy="365040"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -7746,9 +7746,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>3960</xdr:colOff>
+      <xdr:colOff>3240</xdr:colOff>
       <xdr:row>197</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7758,7 +7758,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="527040" y="35934480"/>
-          <a:ext cx="3489840" cy="498960"/>
+          <a:ext cx="3489120" cy="498240"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -7816,9 +7816,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>175320</xdr:colOff>
+      <xdr:colOff>174600</xdr:colOff>
       <xdr:row>197</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7828,7 +7828,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4765320" y="35928000"/>
-          <a:ext cx="3436200" cy="492840"/>
+          <a:ext cx="3435480" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -7888,7 +7888,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>187560</xdr:colOff>
       <xdr:row>195</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:rowOff>142560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7898,7 +7898,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2193480" y="35369280"/>
-          <a:ext cx="360" cy="682920"/>
+          <a:ext cx="360" cy="682200"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7945,9 +7945,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>185040</xdr:colOff>
+      <xdr:colOff>184320</xdr:colOff>
       <xdr:row>190</xdr:row>
-      <xdr:rowOff>10080</xdr:rowOff>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7957,7 +7957,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2187360" y="34632720"/>
-          <a:ext cx="3960" cy="365760"/>
+          <a:ext cx="3240" cy="365040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7998,15 +7998,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>185040</xdr:colOff>
+      <xdr:colOff>184320</xdr:colOff>
       <xdr:row>192</xdr:row>
       <xdr:rowOff>12600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>182520</xdr:colOff>
+      <xdr:colOff>181080</xdr:colOff>
       <xdr:row>195</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8015,8 +8015,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2191320" y="35369280"/>
-          <a:ext cx="4261680" cy="556200"/>
+          <a:off x="2190600" y="35369280"/>
+          <a:ext cx="4260960" cy="555480"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -8052,9 +8052,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>175320</xdr:colOff>
+      <xdr:colOff>174600</xdr:colOff>
       <xdr:row>201</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8064,7 +8064,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="527040" y="36664920"/>
-          <a:ext cx="3410640" cy="492840"/>
+          <a:ext cx="3409920" cy="492120"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartProcess">
           <a:avLst/>
@@ -8116,15 +8116,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>197</xdr:row>
       <xdr:rowOff>158760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>11160</xdr:colOff>
+      <xdr:colOff>9720</xdr:colOff>
       <xdr:row>199</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>15840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8133,8 +8133,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2258280" y="36435960"/>
-          <a:ext cx="10080" cy="226440"/>
+          <a:off x="2257560" y="36435960"/>
+          <a:ext cx="9360" cy="225720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8181,9 +8181,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>35640</xdr:colOff>
+      <xdr:colOff>34920</xdr:colOff>
       <xdr:row>200</xdr:row>
-      <xdr:rowOff>80280</xdr:rowOff>
+      <xdr:rowOff>79560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8193,7 +8193,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="527040" y="36185400"/>
-          <a:ext cx="10080" cy="724680"/>
+          <a:ext cx="9360" cy="723960"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -8225,13 +8225,13 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>6480</xdr:colOff>
       <xdr:row>196</xdr:row>
-      <xdr:rowOff>79560</xdr:rowOff>
+      <xdr:rowOff>78840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>248040</xdr:colOff>
+      <xdr:colOff>247320</xdr:colOff>
       <xdr:row>196</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8240,8 +8240,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4019400" y="36172800"/>
-          <a:ext cx="743400" cy="6840"/>
+          <a:off x="4019400" y="36172080"/>
+          <a:ext cx="742680" cy="6120"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8293,9 +8293,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>746640</xdr:colOff>
+      <xdr:colOff>745920</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>165960</xdr:rowOff>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8309,7 +8309,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="2393640"/>
-          <a:ext cx="3923280" cy="2376000"/>
+          <a:ext cx="3922560" cy="2375280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8330,9 +8330,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>139320</xdr:colOff>
+      <xdr:colOff>138600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8346,7 +8346,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="4971960"/>
-          <a:ext cx="7062480" cy="2653560"/>
+          <a:ext cx="7061760" cy="2652840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8367,9 +8367,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>162720</xdr:colOff>
+      <xdr:colOff>162000</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:rowOff>41040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8383,7 +8383,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="4088880" cy="2435400"/>
+          <a:ext cx="4088160" cy="2434680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8404,9 +8404,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>19440</xdr:colOff>
+      <xdr:colOff>18720</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>80640</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8420,7 +8420,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="7967160"/>
-          <a:ext cx="6193440" cy="3346560"/>
+          <a:ext cx="6192720" cy="3345840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8441,9 +8441,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>29160</xdr:colOff>
+      <xdr:colOff>28440</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>16200</xdr:rowOff>
+      <xdr:rowOff>15480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8457,7 +8457,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="11519640"/>
-          <a:ext cx="4704480" cy="3044160"/>
+          <a:ext cx="4703760" cy="3043440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8478,9 +8478,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>29160</xdr:colOff>
+      <xdr:colOff>28440</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8494,7 +8494,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="14635440"/>
-          <a:ext cx="4704480" cy="2855160"/>
+          <a:ext cx="4703760" cy="2854440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8515,9 +8515,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>467280</xdr:colOff>
+      <xdr:colOff>466560</xdr:colOff>
       <xdr:row>109</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8531,7 +8531,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="17766000"/>
-          <a:ext cx="8139960" cy="2429640"/>
+          <a:ext cx="8139240" cy="2428920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8552,9 +8552,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>181800</xdr:colOff>
+      <xdr:colOff>181080</xdr:colOff>
       <xdr:row>126</xdr:row>
-      <xdr:rowOff>168120</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8568,7 +8568,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="20464920"/>
-          <a:ext cx="6355800" cy="2905920"/>
+          <a:ext cx="6355080" cy="2905200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8589,9 +8589,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>486360</xdr:colOff>
+      <xdr:colOff>485640</xdr:colOff>
       <xdr:row>152</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8605,7 +8605,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="23548320"/>
-          <a:ext cx="5910840" cy="4620240"/>
+          <a:ext cx="5910120" cy="4619520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8631,7 +8631,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
+      <xdr:colOff>9360</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:to>
@@ -8643,7 +8643,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1024200" y="3835080"/>
-          <a:ext cx="1222200" cy="360"/>
+          <a:ext cx="1221480" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8686,13 +8686,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>590400</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>587880</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:colOff>587160</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8701,8 +8701,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3723840" y="2181240"/>
-          <a:ext cx="747000" cy="3960"/>
+          <a:off x="3723840" y="2180520"/>
+          <a:ext cx="746280" cy="3240"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8745,13 +8745,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>6480</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>162360</xdr:rowOff>
+      <xdr:rowOff>161640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>3960</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:colOff>3240</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>164880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8760,8 +8760,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3889440" y="1851120"/>
-          <a:ext cx="746640" cy="3960"/>
+          <a:off x="3889440" y="1850400"/>
+          <a:ext cx="745920" cy="3240"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8804,13 +8804,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>746640</xdr:colOff>
+      <xdr:colOff>745920</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8819,8 +8819,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3882960" y="1514520"/>
-          <a:ext cx="746640" cy="3960"/>
+          <a:off x="3882960" y="1513800"/>
+          <a:ext cx="745920" cy="3240"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8863,13 +8863,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>149400</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>746640</xdr:colOff>
+      <xdr:colOff>745920</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8878,8 +8878,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3882960" y="1012680"/>
-          <a:ext cx="746640" cy="3960"/>
+          <a:off x="3882960" y="1011960"/>
+          <a:ext cx="745920" cy="3240"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8922,13 +8922,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>12600</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>187560</xdr:rowOff>
+      <xdr:rowOff>186840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
+      <xdr:colOff>9360</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>191520</xdr:rowOff>
+      <xdr:rowOff>190080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8937,8 +8937,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3895560" y="187560"/>
-          <a:ext cx="746640" cy="3960"/>
+          <a:off x="3895560" y="186840"/>
+          <a:ext cx="745920" cy="3240"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8985,7 +8985,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:colOff>15840</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>6840</xdr:rowOff>
     </xdr:to>
@@ -8997,7 +8997,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1030680" y="2851200"/>
-          <a:ext cx="1222200" cy="360"/>
+          <a:ext cx="1221480" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9044,7 +9044,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3960</xdr:colOff>
+      <xdr:colOff>3240</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
@@ -9056,7 +9056,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="878040" y="3263760"/>
-          <a:ext cx="1362240" cy="360"/>
+          <a:ext cx="1361520" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9103,7 +9103,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3960</xdr:colOff>
+      <xdr:colOff>3240</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
@@ -9115,7 +9115,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="878040" y="4489200"/>
-          <a:ext cx="1362240" cy="360"/>
+          <a:ext cx="1361520" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9158,13 +9158,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>6480</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>150120</xdr:rowOff>
+      <xdr:rowOff>149400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1209600</xdr:colOff>
+      <xdr:colOff>1208880</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9173,8 +9173,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1030680" y="6462000"/>
-          <a:ext cx="1203120" cy="10080"/>
+          <a:off x="1030680" y="6461280"/>
+          <a:ext cx="1202400" cy="9360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9221,7 +9221,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
+      <xdr:colOff>9360</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>95760</xdr:rowOff>
     </xdr:to>
@@ -9233,7 +9233,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1024200" y="5581800"/>
-          <a:ext cx="1222200" cy="360"/>
+          <a:ext cx="1221480" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9280,7 +9280,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>10080</xdr:colOff>
+      <xdr:colOff>9360</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
@@ -9292,7 +9292,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1024200" y="4070160"/>
-          <a:ext cx="1222200" cy="360"/>
+          <a:ext cx="1221480" cy="360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -14578,8 +14578,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E60" activeCellId="0" sqref="E60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>